<commit_message>
this verison is working
</commit_message>
<xml_diff>
--- a/Files/Config.xlsx
+++ b/Files/Config.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\somep\Documents\UiPath\Git\Dice\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892543AB-ED3B-484C-8661-4F95EFD683A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99BED69-FA09-4647-BFAF-FE6406CF0D3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="raj" sheetId="1" r:id="rId1"/>
-    <sheet name="swathi" sheetId="2" r:id="rId2"/>
+    <sheet name="swathi" sheetId="2" r:id="rId1"/>
+    <sheet name="raj" sheetId="1" r:id="rId2"/>
+    <sheet name="Backup" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>srajrsraj@gmail.com</t>
   </si>
@@ -71,6 +72,9 @@
   </si>
   <si>
     <t>20105/27560/75024/36101/99801/85001/72201/94203/80201/06101/19901/20001/32301/30301/96801/83701/62701/46201/50301/66601/40601/70801/04330/21401/02108/48901/55101/39201/65101/59601/68501/89701/03301/08601/87501/12201/27601/58501/43201/73101/93701/17101/02901/29201/37201/73301/84101/05601/23218/98501/25301</t>
+  </si>
+  <si>
+    <t>27560/75024/36101/99801/85001/72201/94203/80201/06101/19901/20001/32301/30301/96801/83701/62701/46201/50301/66601/40601/70801/04330/21401/02108/48901/55101/39201/65101/59601/68501/89701/03301/08601/87501/12201/27601/58501/43201/73101/93701/17101/02901/29201/37201/73301/84101/05601/23218/98501/25301</t>
   </si>
 </sst>
 </file>
@@ -388,11 +392,84 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2837E4FD-75ED-4B17-B393-F97D74428759}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +521,7 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -467,72 +544,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2837E4FD-75ED-4B17-B393-F97D74428759}">
-  <dimension ref="A1:I2"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6475804-69CD-4079-960C-25F0052843DA}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
         <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>